<commit_message>
Updated for GitHub Pages: removed server dependency, added local storage, fixed file paths
</commit_message>
<xml_diff>
--- a/Team Roster.xlsx
+++ b/Team Roster.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Code Hero\Leaderboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C6E4D8-8AB3-46AF-A58B-16B6B30292B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E7DBAF6-23A1-4F24-AC5A-E8C766766469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5F0416C3-331E-4E4B-89B4-263777EE6164}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{628B9F55-6E98-4901-A3A3-B30F95546C8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>BTFD</t>
+  </si>
   <si>
     <t>Garrett Brigman</t>
   </si>
@@ -42,80 +66,56 @@
     <t>John Mueller</t>
   </si>
   <si>
+    <t>Master Market Jedi's</t>
+  </si>
+  <si>
     <t>Mike Honkamp</t>
   </si>
   <si>
     <t>Brian Lehky</t>
   </si>
   <si>
-    <t xml:space="preserve">Steve Jaeger </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alton Wigly </t>
+    <t>Leverage Legends</t>
+  </si>
+  <si>
+    <t>Steve Jaeger</t>
+  </si>
+  <si>
+    <t>Alton Wigly</t>
+  </si>
+  <si>
+    <t>Cap Gains Gang</t>
+  </si>
+  <si>
+    <t>Perry Pocaro</t>
   </si>
   <si>
     <t>Jim Mirsberger</t>
-  </si>
-  <si>
-    <t>Players</t>
-  </si>
-  <si>
-    <t>Teams</t>
-  </si>
-  <si>
-    <t>https://www.danainvestment.com/team-member/michael-honkamp-cfa/</t>
-  </si>
-  <si>
-    <t>https://www.danainvestment.com/team-member/brian-lehky/</t>
-  </si>
-  <si>
-    <t>https://www.danainvestment.com/team-member/john-mueller/</t>
-  </si>
-  <si>
-    <t>https://www.danainvestment.com/team-member/alton-weigley-cfa/</t>
-  </si>
-  <si>
-    <t>https://www.danainvestment.com/team-member/perry-porcaro/</t>
-  </si>
-  <si>
-    <t>Perry Pocaro</t>
-  </si>
-  <si>
-    <t>https://www.danainvestment.com/team-member/steve-jaeger-cfp/</t>
-  </si>
-  <si>
-    <t>https://www.danainvestment.com/team-member/garrett-j-brigman/</t>
-  </si>
-  <si>
-    <t>https://www.danainvestment.com/team-member/mark-mirsberger-cpa/</t>
-  </si>
-  <si>
-    <t>Player Bio</t>
-  </si>
-  <si>
-    <t>BTFD</t>
-  </si>
-  <si>
-    <t>Leverage Legends</t>
-  </si>
-  <si>
-    <t>Cap Gains Gang</t>
-  </si>
-  <si>
-    <t>Master Market Jedi's</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,7 +126,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -134,12 +134,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,118 +474,141 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B51807-E812-4B71-9B6F-2C26D70B9966}">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EED55F6-EF50-4CB0-B751-088E2CC8CD6B}">
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection sqref="A1:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>